<commit_message>
Fixed, fill closed manuc now working
</commit_message>
<xml_diff>
--- a/CSV/manufacturers_locations.xlsx
+++ b/CSV/manufacturers_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsmagnusjohnsen/Documents/Masteroppgave/StructuralCircle/structuralCircle/CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562CD6AE-BA7E-A941-86CE-71C7A9260F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1D4DA6-31F0-0540-97ED-8EFA8461839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="-7500" windowWidth="38400" windowHeight="23500" xr2:uid="{1D182BFB-3642-2D47-A43C-A3B60F7294D7}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>10.476661</t>
   </si>
   <si>
-    <t>Tree</t>
-  </si>
-  <si>
     <t>63.368923</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Byggmakker</t>
+  </si>
+  <si>
+    <t>Timber</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,7 +479,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -490,13 +490,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -507,13 +507,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -524,13 +524,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -541,19 +541,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some plotting of maps for overleaf
</commit_message>
<xml_diff>
--- a/CSV/manufacturers_locations.xlsx
+++ b/CSV/manufacturers_locations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larsmagnusjohnsen/Documents/Masteroppgave/StructuralCircle/structuralCircle/CSV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9d71f9bda8fdeb6/Dokumenter/NTNU notater/10.semester/Masteroppgave^J Sigurd og Lars/structuralCircle/CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6FE6-94F4-B948-A403-CA0D6052C04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-7500" windowWidth="38400" windowHeight="23500" xr2:uid="{1D182BFB-3642-2D47-A43C-A3B60F7294D7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D182BFB-3642-2D47-A43C-A3B60F7294D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -453,14 +453,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13866D7C-753B-B44A-B944-2206441C585E}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -488,7 +490,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -502,7 +504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -516,7 +518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Started on case study for conference
</commit_message>
<xml_diff>
--- a/CSV/manufacturers_locations.xlsx
+++ b/CSV/manufacturers_locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9d71f9bda8fdeb6/Dokumenter/NTNU notater/10.semester/Masteroppgave^J Sigurd og Lars/structuralCircle/CSV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303B6FE6-94F4-B948-A403-CA0D6052C04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{303B6FE6-94F4-B948-A403-CA0D6052C04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{652E60CD-FF1B-4BE5-8F65-E9C9F240C587}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1D182BFB-3642-2D47-A43C-A3B60F7294D7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Byggmakker Tiller</t>
+  </si>
+  <si>
+    <t>GSM Industrial</t>
+  </si>
+  <si>
+    <t>53.493746</t>
+  </si>
+  <si>
+    <t>-2.2086889</t>
   </si>
 </sst>
 </file>
@@ -133,10 +142,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,6 +162,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -451,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13866D7C-753B-B44A-B944-2206441C585E}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -532,6 +546,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>